<commit_message>
add access product via search bar test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="wrong-login-data" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="search-input-data" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,18 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>email</t>
+    <t>searchInput</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>wrongemail@gmail.com</t>
-  </si>
-  <si>
-    <t>wrongemail123</t>
+    <t>MacBook</t>
   </si>
 </sst>
 </file>
@@ -278,24 +272,15 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="20.13"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>